<commit_message>
-Sparql abfragen in doc extrahiert -testdata update -grapf von instanzen -graph von ontologie
Signed-off-by: NonSense86 <nonsense86@gmail.com>
</commit_message>
<xml_diff>
--- a/abgabe1/doc/testdata.xlsx
+++ b/abgabe1/doc/testdata.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
   <si>
     <t>Abfrage</t>
   </si>
@@ -143,43 +142,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="3">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,7 +171,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -199,76 +179,329 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="165">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="20"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal" xfId="20"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="1" customBuiltin="1"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:IW25"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.6235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9294117647059"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.9960784313725"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="69.2901960784314"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="10.8078431372549"/>
+    <col min="1" max="1" width="39.5703125" style="1"/>
+    <col min="2" max="2" width="13.85546875" style="1"/>
+    <col min="3" max="3" width="13.5703125" style="1"/>
+    <col min="4" max="4" width="15" style="1"/>
+    <col min="5" max="5" width="69.28515625" style="1"/>
+    <col min="6" max="257" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="2">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -285,92 +518,92 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="2">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="3">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="4">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="5">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="6">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="7">
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -380,14 +613,14 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="8">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -397,14 +630,14 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="9">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -414,14 +647,14 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="10">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -431,14 +664,14 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="11">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -448,14 +681,14 @@
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="12">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -465,14 +698,14 @@
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="13">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -482,14 +715,14 @@
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="14">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
@@ -499,14 +732,14 @@
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="15">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -516,14 +749,14 @@
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="16">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -533,14 +766,14 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="17">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -550,14 +783,14 @@
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="18">
+    <row r="18" spans="1:5" ht="30">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -567,14 +800,14 @@
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="1">
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="19">
+    <row r="19" spans="1:5" ht="45">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -584,14 +817,14 @@
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="20">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
@@ -601,14 +834,14 @@
       <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="21">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
@@ -618,14 +851,14 @@
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="22">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
@@ -635,87 +868,98 @@
       <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="23">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:IW1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.8078431372549"/>
+    <col min="1" max="257" width="10.85546875" style="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:IW1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.8078431372549"/>
+    <col min="1" max="257" width="10.85546875" style="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>